<commit_message>
Fix container name issue
</commit_message>
<xml_diff>
--- a/wheel_post_processing/packages_to_process_non_noarch-testing.xlsx
+++ b/wheel_post_processing/packages_to_process_non_noarch-testing.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">param-2.0.1-py3-none-any.whl</t>
   </si>
   <si>
-    <t xml:space="preserve">‘NoArch</t>
+    <t xml:space="preserve">3.9</t>
   </si>
   <si>
     <t xml:space="preserve">quick_run</t>
@@ -322,7 +322,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>